<commit_message>
adding the pcibex version of the randomized video list.
</commit_message>
<xml_diff>
--- a/bad_item_pairings.xlsx
+++ b/bad_item_pairings.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abima\Documents\Penn\adult-matching-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26324671-852D-4D9A-80DF-40D1DED1D587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31409CA-FDCE-42A4-939B-06F04C192AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9150" yWindow="660" windowWidth="21765" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="asl_sym_ratings_with_bad_predic" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>class</t>
   </si>
@@ -977,10 +978,13 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1245,9 +1249,6 @@
       <c r="D18">
         <v>1.05232926</v>
       </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1261,9 +1262,6 @@
       </c>
       <c r="D19">
         <v>0.785718904</v>
-      </c>
-      <c r="E19" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>